<commit_message>
cost per lead calculation
</commit_message>
<xml_diff>
--- a/Business Metrics & Modeling/Business Metrics.xlsx
+++ b/Business Metrics & Modeling/Business Metrics.xlsx
@@ -8,22 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Click Through Rate" sheetId="2" r:id="rId1"/>
-    <sheet name="Cost Per Click" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Cost Per Click - Costs Per Lead" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Source Platform</t>
   </si>
   <si>
-    <t>CPC Formula</t>
-  </si>
-  <si>
     <t>FB Ad</t>
   </si>
   <si>
@@ -49,6 +45,12 @@
   </si>
   <si>
     <t>FB Ads</t>
+  </si>
+  <si>
+    <t>Costs Per Lead (CPL)</t>
+  </si>
+  <si>
+    <t>Total Leads</t>
   </si>
 </sst>
 </file>
@@ -82,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,12 +112,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -408,30 +417,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1100</v>
@@ -446,7 +457,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2000</v>
@@ -461,7 +472,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1500</v>
@@ -481,95 +492,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
-        <v>1500</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3000</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>700</v>
+      </c>
+      <c r="C4">
+        <v>1900</v>
+      </c>
+      <c r="D4">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>700</v>
-      </c>
-      <c r="D4">
-        <v>1900</v>
-      </c>
-      <c r="E4">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <f>C3/C4</f>
+      <c r="B6" s="3">
+        <f>B3/B4</f>
         <v>2.1428571428571428</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" ref="D5:E5" si="0">D3/D4</f>
+      <c r="C6" s="3">
+        <f t="shared" ref="C6:D6" si="0">C3/C4</f>
         <v>1.5789473684210527</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>1.0010010010010011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B3/B8</f>
+        <v>93.75</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ref="C9:D9" si="1">C3/C8</f>
+        <v>47.61904761904762</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>44.642857142857146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Customer acquisition cost, optimizing coversion funnel, cost per acquisition
</commit_message>
<xml_diff>
--- a/Business Metrics & Modeling/Business Metrics.xlsx
+++ b/Business Metrics & Modeling/Business Metrics.xlsx
@@ -4,18 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Click Through Rate" sheetId="2" r:id="rId1"/>
     <sheet name="Cost Per Click - Costs Per Lead" sheetId="1" r:id="rId2"/>
+    <sheet name="Customer Acuquistion Cost" sheetId="3" r:id="rId3"/>
+    <sheet name="CAC - Average" sheetId="4" r:id="rId4"/>
+    <sheet name="Optimizing Marketing Funnel" sheetId="5" r:id="rId5"/>
+    <sheet name="Example Conversion Rate Chart" sheetId="6" r:id="rId6"/>
+    <sheet name="Cost Per Acquisition" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Source Platform</t>
   </si>
@@ -51,16 +56,120 @@
   </si>
   <si>
     <t>Total Leads</t>
+  </si>
+  <si>
+    <t>Marketing Cost</t>
+  </si>
+  <si>
+    <t>Sales &amp; Marketing Salaries</t>
+  </si>
+  <si>
+    <t>Overhead Cost for Sales &amp; Marketing</t>
+  </si>
+  <si>
+    <t>Total Sales &amp; Marketing Costs</t>
+  </si>
+  <si>
+    <t>Number of Paid Customers</t>
+  </si>
+  <si>
+    <t>Customer Acquisition Cost (CAC)</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>When customer takes time to convert, we need to average those CAC across those months.</t>
+  </si>
+  <si>
+    <t>Example: Customer is on trial, then converted to paid customer.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sales Cycle is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 months</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Conversions Rate 
+based on Impression</t>
+  </si>
+  <si>
+    <t>Conversions Rate 
+based on each Level</t>
+  </si>
+  <si>
+    <t>Arrived on site</t>
+  </si>
+  <si>
+    <t>Downloaded brochure</t>
+  </si>
+  <si>
+    <t>Added items to cart</t>
+  </si>
+  <si>
+    <t>Purchased items</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Conversion Rates</t>
+  </si>
+  <si>
+    <t>Number of Leads (Non Paying Customers)</t>
+  </si>
+  <si>
+    <t>(can get it form Cost Per Lead stage)</t>
+  </si>
+  <si>
+    <t>Cost Per Acquisiton (Non Paying Customers)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +188,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,13 +228,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -128,6 +252,202 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Example Conversion Rate Chart'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conversion Rates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Example Conversion Rate Chart'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Example Conversion Rate Chart'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.51968929338975056</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28308588738224438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74302749040602212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96994468998869898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18048238772009295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69256369419309349</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1870679772644053E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69702458519995592</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5775072004984523E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6727428942462419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.43499916308087871</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.34973546395697497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="57635200"/>
+        <c:axId val="57636736"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="57635200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm-yy" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57636736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="57636736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57635200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,4 +925,586 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>25000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SUM(B2:B4)</f>
+        <v>35500</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:D6" si="0">SUM(C2:C4)</f>
+        <v>45000</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>38500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>325</v>
+      </c>
+      <c r="D8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6">
+        <f>B6/B8</f>
+        <v>118.33333333333333</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" ref="C9:D9" si="1">C6/C8</f>
+        <v>138.46153846153845</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9500</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>25000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>25000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>325</v>
+      </c>
+      <c r="D12">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <f>(B7+(0.5*(B8+B9)+(0.5*(C8+C9))))/C12</f>
+        <v>120</v>
+      </c>
+      <c r="D13" s="6">
+        <f>(C7+(0.5*(C8+C9)+(0.5*(D8+D9))))/D12</f>
+        <v>129.28571428571428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>430</v>
+      </c>
+      <c r="C5" s="10">
+        <f>B5/$B$3</f>
+        <v>0.43</v>
+      </c>
+      <c r="D5" s="9">
+        <f>B5/B3</f>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>193</v>
+      </c>
+      <c r="C6" s="10">
+        <f>B6/$B$3</f>
+        <v>0.193</v>
+      </c>
+      <c r="D6" s="9">
+        <f>B6/B5</f>
+        <v>0.44883720930232557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+      <c r="C7" s="10">
+        <f>B7/$B$3</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D7" s="9">
+        <f>B7/B6</f>
+        <v>0.38860103626943004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>0.51968929338975056</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11">
+        <v>43862</v>
+      </c>
+      <c r="B3">
+        <v>0.28308588738224438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11">
+        <v>43891</v>
+      </c>
+      <c r="B4">
+        <v>0.74302749040602212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11">
+        <v>43922</v>
+      </c>
+      <c r="B5">
+        <v>0.96994468998869898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11">
+        <v>43952</v>
+      </c>
+      <c r="B6">
+        <v>0.18048238772009295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="11">
+        <v>43983</v>
+      </c>
+      <c r="B7">
+        <v>0.69256369419309349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="11">
+        <v>44013</v>
+      </c>
+      <c r="B8">
+        <v>7.1870679772644053E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="11">
+        <v>44044</v>
+      </c>
+      <c r="B9">
+        <v>0.69702458519995592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="11">
+        <v>44075</v>
+      </c>
+      <c r="B10">
+        <v>2.5775072004984523E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="11">
+        <v>44105</v>
+      </c>
+      <c r="B11">
+        <v>0.6727428942462419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="11">
+        <v>44136</v>
+      </c>
+      <c r="B12">
+        <v>0.43499916308087871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="11">
+        <v>44166</v>
+      </c>
+      <c r="B13">
+        <v>0.34973546395697497</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>25000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6">
+        <f>SUM(B2:B4)</f>
+        <v>35500</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" ref="C6:D6" si="0">SUM(C2:C4)</f>
+        <v>45000</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>38500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>191</v>
+      </c>
+      <c r="C8">
+        <v>135</v>
+      </c>
+      <c r="D8">
+        <v>130</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="6">
+        <f>B6/B8</f>
+        <v>185.86387434554973</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" ref="C9:D9" si="1">C6/C8</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>296.15384615384613</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>